<commit_message>
Added BCSRIF list of projects
</commit_message>
<xml_diff>
--- a/science_projects schema.xlsx
+++ b/science_projects schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ennsj\Documents\2. PSSI\Salmon Science Wrap-up Series\salmon_science_wrap-up_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4628F5-7E79-4DC1-BAED-892E4F1C3275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F122B8-51DC-4C02-B283-A6A41A583D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1485" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{45EABC72-8870-4B2F-BA00-4F0CB2CAC457}"/>
   </bookViews>
@@ -1145,7 +1145,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Keeping projects to unique project_id only
</commit_message>
<xml_diff>
--- a/science_projects schema.xlsx
+++ b/science_projects schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ennsj\Documents\2. PSSI\Salmon Science Wrap-up Series\salmon_science_wrap-up_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F122B8-51DC-4C02-B283-A6A41A583D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F728EF31-0CF5-4701-87CB-DA9AC1F8E51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1485" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{45EABC72-8870-4B2F-BA00-4F0CB2CAC457}"/>
+    <workbookView xWindow="-28920" yWindow="1485" windowWidth="29040" windowHeight="15720" xr2:uid="{45EABC72-8870-4B2F-BA00-4F0CB2CAC457}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
   <si>
     <t>Fiscal year</t>
   </si>
@@ -283,6 +283,48 @@
 •	project.export..long., Science.PSSI.Projects, and Speaker.Themes  are all joined by the column project_id,
 •	Speaker.Themes and session_info are joined by the column session.
 </t>
+  </si>
+  <si>
+    <t>BCSRIF.Project.List.September.2025</t>
+  </si>
+  <si>
+    <t>Project Number</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Type of Organization (Account) (Account)</t>
+  </si>
+  <si>
+    <t>Geographic Distribution</t>
+  </si>
+  <si>
+    <t>Location of project</t>
+  </si>
+  <si>
+    <t>Program Pillar</t>
+  </si>
+  <si>
+    <t>Agreement Start Date</t>
+  </si>
+  <si>
+    <t>Agreement End Date</t>
+  </si>
+  <si>
+    <t>Description Short</t>
+  </si>
+  <si>
+    <t>List of Partners or Collaborators</t>
+  </si>
+  <si>
+    <t>Species Group</t>
   </si>
 </sst>
 </file>
@@ -330,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -343,11 +385,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -380,28 +434,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8B84CFB-ECD7-4585-98A8-9BDA56364EA5}" name="Table1" displayName="Table1" ref="B2:B54" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8B84CFB-ECD7-4585-98A8-9BDA56364EA5}" name="Table1" displayName="Table1" ref="B2:B54" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B2:B54" xr:uid="{D8B84CFB-ECD7-4585-98A8-9BDA56364EA5}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{4366194B-F2C2-4B00-8F60-5F246F168365}" name="project.export..long." dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{4366194B-F2C2-4B00-8F60-5F246F168365}" name="project.export..long." dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E7B1A6E-37E7-4481-97C0-55EDA3016F4F}" name="Table2" displayName="Table2" ref="D2:D28" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E7B1A6E-37E7-4481-97C0-55EDA3016F4F}" name="Table2" displayName="Table2" ref="D2:D28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="D2:D28" xr:uid="{6E7B1A6E-37E7-4481-97C0-55EDA3016F4F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B0EF64DD-3714-4A15-9CFA-41643C659D3D}" name="Science.PSSI.Projects" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B0EF64DD-3714-4A15-9CFA-41643C659D3D}" name="Science.PSSI.Projects" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D42A271-A7CE-44ED-8500-0C543399B313}" name="Table3" displayName="Table3" ref="F2:F6" totalsRowShown="0">
-  <autoFilter ref="F2:F6" xr:uid="{3D42A271-A7CE-44ED-8500-0C543399B313}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D42A271-A7CE-44ED-8500-0C543399B313}" name="Table3" displayName="Table3" ref="H2:H6" totalsRowShown="0">
+  <autoFilter ref="H2:H6" xr:uid="{3D42A271-A7CE-44ED-8500-0C543399B313}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{12D9A6FD-4AA9-485D-92F5-099C712AD603}" name="Speaker.Themes"/>
   </tableColumns>
@@ -410,10 +464,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88DE97A0-296F-4E94-B3D2-45414657DA82}" name="Table4" displayName="Table4" ref="H2:H5" totalsRowShown="0">
-  <autoFilter ref="H2:H5" xr:uid="{88DE97A0-296F-4E94-B3D2-45414657DA82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88DE97A0-296F-4E94-B3D2-45414657DA82}" name="Table4" displayName="Table4" ref="J2:J5" totalsRowShown="0">
+  <autoFilter ref="J2:J5" xr:uid="{88DE97A0-296F-4E94-B3D2-45414657DA82}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{FE846E16-7490-4F6D-8F0F-04602B29FA56}" name="session_info"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{10036D84-79B7-4CC9-9586-61AF4F60B8F0}" name="Table5" displayName="Table5" ref="F2:F15" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="F2:F15" xr:uid="{10036D84-79B7-4CC9-9586-61AF4F60B8F0}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{006106E9-7CC4-4B8F-B887-51E658EE6FCE}" name="BCSRIF.Project.List.September.2025" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450C169A-AAC2-41A3-85C2-7895BBCDD81E}">
-  <dimension ref="B2:H54"/>
+  <dimension ref="B2:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,152 +811,197 @@
     <col min="2" max="2" width="45.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="4.1796875" customWidth="1"/>
     <col min="4" max="4" width="27.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.90625" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="4.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" customWidth="1"/>
+    <col min="9" max="9" width="4.453125" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
         <v>71</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F7" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F9" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F10" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F11" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F13" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F14" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1131,11 +1240,12 @@
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri"&amp;12&amp;K000000 Unclassified - Non-Classifié&amp;1#_x000D_</oddHeader>
   </headerFooter>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1144,7 +1254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC58E8A0-DAC6-4285-8662-9D262E72BB0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>